<commit_message>
Update excel and payrollv6
</commit_message>
<xml_diff>
--- a/Data_Gaji_Karyawan.xlsx
+++ b/Data_Gaji_Karyawan.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9947ADD8-F6DD-4351-AC8D-A5869562B7D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="245" yWindow="14" windowWidth="16098" windowHeight="9659" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Periode</t>
   </si>
@@ -64,12 +70,39 @@
     <t>Mei 2025</t>
   </si>
   <si>
-    <t>Karyawan 1</t>
-  </si>
-  <si>
     <t>Karyawan 2</t>
   </si>
   <si>
+    <t>Karyawan 7</t>
+  </si>
+  <si>
+    <t>100001</t>
+  </si>
+  <si>
+    <t>100002</t>
+  </si>
+  <si>
+    <t>100007</t>
+  </si>
+  <si>
+    <t>100008</t>
+  </si>
+  <si>
+    <t>Sapto Wahyu Sudrajat Bin Misyanto</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Terlambat</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>mtvgsapto@gmail.com</t>
+  </si>
+  <si>
     <t>Karyawan 3</t>
   </si>
   <si>
@@ -82,53 +115,29 @@
     <t>Karyawan 6</t>
   </si>
   <si>
-    <t>Karyawan 7</t>
-  </si>
-  <si>
-    <t>Karyawan 8</t>
-  </si>
-  <si>
-    <t>Karyawan 9</t>
-  </si>
-  <si>
-    <t>Karyawan 10</t>
-  </si>
-  <si>
-    <t>100001</t>
-  </si>
-  <si>
-    <t>100002</t>
-  </si>
-  <si>
-    <t>100003</t>
-  </si>
-  <si>
-    <t>100004</t>
-  </si>
-  <si>
-    <t>100005</t>
-  </si>
-  <si>
-    <t>100006</t>
-  </si>
-  <si>
-    <t>100007</t>
-  </si>
-  <si>
-    <t>100008</t>
-  </si>
-  <si>
-    <t>100009</t>
-  </si>
-  <si>
-    <t>100010</t>
+    <t>faishalfh1@gmail.com</t>
+  </si>
+  <si>
+    <t>ntvgsapto@gmail.com</t>
+  </si>
+  <si>
+    <t>otvgsapto@gmail.com</t>
+  </si>
+  <si>
+    <t>ztvgsapto@gmail.com</t>
+  </si>
+  <si>
+    <t>ptvgsapto@gmail.com</t>
+  </si>
+  <si>
+    <t>vivihandayani2405@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +149,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,20 +194,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -237,7 +265,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,9 +297,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,6 +349,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,14 +542,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,516 +570,456 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
         <v>20</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>4000000</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>200000</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>150000</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>500000</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>300000</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>5150000</v>
       </c>
-      <c r="K2">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>30000</v>
+      </c>
+      <c r="N2">
         <v>50000</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>200000</v>
       </c>
-      <c r="M2">
+      <c r="P2">
         <v>100000</v>
       </c>
-      <c r="N2">
+      <c r="Q2">
         <v>350000</v>
       </c>
-      <c r="O2">
+      <c r="R2">
         <v>4800000</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
         <v>22</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4200000</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>220000</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>100000</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>600000</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>350000</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>5470000</v>
       </c>
-      <c r="K3">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>40000</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>210000</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>90000</v>
       </c>
-      <c r="N3">
+      <c r="Q3">
         <v>340000</v>
       </c>
-      <c r="O3">
+      <c r="R3">
         <v>5130000</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
       </c>
       <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
         <v>3900000</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>180000</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>120000</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>400000</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>250000</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>4850000</v>
       </c>
-      <c r="K4">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>60000</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>190000</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <v>110000</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
         <v>360000</v>
       </c>
-      <c r="O4">
+      <c r="R4">
         <v>4490000</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>4500000</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>210000</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>130000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>550000</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>320000</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5710000</v>
       </c>
-      <c r="K5">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
         <v>30000</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>220000</v>
       </c>
-      <c r="M5">
+      <c r="P5">
         <v>95000</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
         <v>345000</v>
       </c>
-      <c r="O5">
+      <c r="R5">
         <v>5365000</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6">
-        <v>23</v>
-      </c>
-      <c r="E6">
+      <c r="F6">
         <v>4600000</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>230000</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>110000</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>580000</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>330000</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5850000</v>
       </c>
-      <c r="K6">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>20000</v>
       </c>
-      <c r="L6">
+      <c r="O6">
         <v>230000</v>
       </c>
-      <c r="M6">
+      <c r="P6">
         <v>85000</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
         <v>335000</v>
       </c>
-      <c r="O6">
+      <c r="R6">
         <v>5515000</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7">
+        <v>22</v>
+      </c>
+      <c r="F7">
         <v>4000000</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>190000</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>100000</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>520000</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>300000</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>5110000</v>
       </c>
-      <c r="K7">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
         <v>50000</v>
       </c>
-      <c r="L7">
+      <c r="O7">
         <v>200000</v>
       </c>
-      <c r="M7">
+      <c r="P7">
         <v>105000</v>
       </c>
-      <c r="N7">
+      <c r="Q7">
         <v>355000</v>
       </c>
-      <c r="O7">
+      <c r="R7">
         <v>4755000</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
       <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
         <v>4100000</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>200000</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>125000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>500000</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>310000</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>5235000</v>
       </c>
-      <c r="K8">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
         <v>45000</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <v>210000</v>
       </c>
-      <c r="M8">
+      <c r="P8">
         <v>100000</v>
       </c>
-      <c r="N8">
+      <c r="Q8">
         <v>355000</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <v>4880000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>4200000</v>
-      </c>
-      <c r="F9">
-        <v>220000</v>
-      </c>
-      <c r="G9">
-        <v>135000</v>
-      </c>
-      <c r="H9">
-        <v>610000</v>
-      </c>
-      <c r="I9">
-        <v>340000</v>
-      </c>
-      <c r="J9">
-        <v>5505000</v>
-      </c>
-      <c r="K9">
-        <v>35000</v>
-      </c>
-      <c r="L9">
-        <v>220000</v>
-      </c>
-      <c r="M9">
-        <v>92000</v>
-      </c>
-      <c r="N9">
-        <v>347000</v>
-      </c>
-      <c r="O9">
-        <v>5158000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10">
-        <v>21</v>
-      </c>
-      <c r="E10">
-        <v>4300000</v>
-      </c>
-      <c r="F10">
-        <v>210000</v>
-      </c>
-      <c r="G10">
-        <v>120000</v>
-      </c>
-      <c r="H10">
-        <v>530000</v>
-      </c>
-      <c r="I10">
-        <v>310000</v>
-      </c>
-      <c r="J10">
-        <v>5470000</v>
-      </c>
-      <c r="K10">
-        <v>30000</v>
-      </c>
-      <c r="L10">
-        <v>205000</v>
-      </c>
-      <c r="M10">
-        <v>98000</v>
-      </c>
-      <c r="N10">
-        <v>333000</v>
-      </c>
-      <c r="O10">
-        <v>5137000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>20</v>
-      </c>
-      <c r="E11">
-        <v>4400000</v>
-      </c>
-      <c r="F11">
-        <v>200000</v>
-      </c>
-      <c r="G11">
-        <v>110000</v>
-      </c>
-      <c r="H11">
-        <v>490000</v>
-      </c>
-      <c r="I11">
-        <v>300000</v>
-      </c>
-      <c r="J11">
-        <v>5500000</v>
-      </c>
-      <c r="K11">
-        <v>40000</v>
-      </c>
-      <c r="L11">
-        <v>215000</v>
-      </c>
-      <c r="M11">
-        <v>97000</v>
-      </c>
-      <c r="N11">
-        <v>352000</v>
-      </c>
-      <c r="O11">
-        <v>5148000</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B4D914F1-D3BD-4B0C-A3B5-B0C434726F5B}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{38FB112C-4E0E-49FA-B7EE-E85156A89733}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{4A25FA12-BBB3-49A5-8D1D-554180B58DA0}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{77F6C4A0-F848-4BAD-A7EF-F6559B5BD5F1}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{D5494300-6138-4635-9441-EB4E6EB59712}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{B70CB6CB-C94F-45EB-A73B-81BEA9A7789F}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{0B144C59-5F54-413A-BAEC-A8B1C328B823}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Disabled and Enabled Button
</commit_message>
<xml_diff>
--- a/Data_Gaji_Karyawan.xlsx
+++ b/Data_Gaji_Karyawan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FAISHAL\Documents\payroll_inix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9947ADD8-F6DD-4351-AC8D-A5869562B7D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2299B13-31B2-4E02-9F97-3AA73B44A130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="245" yWindow="14" windowWidth="16098" windowHeight="9659" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,9 +223,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -263,9 +263,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -298,26 +298,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,26 +333,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,26 +509,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -674,7 +640,7 @@
         <v>4800000</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -730,7 +696,7 @@
         <v>5130000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -786,7 +752,7 @@
         <v>4490000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -842,7 +808,7 @@
         <v>5365000</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -898,7 +864,7 @@
         <v>5515000</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -954,7 +920,7 @@
         <v>4755000</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1009,6 +975,9 @@
       <c r="R8">
         <v>4880000</v>
       </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>